<commit_message>
CAN1-68  Configuration Test cases V2
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/configuration _register_test_cases.xlsx
+++ b/Documentations/Test Cases/configuration _register_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hruy1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578D3D91-566D-490E-BBF0-19024D15F396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D1E4C-84C2-4B69-8E77-D98021DC18C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,253 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B9A5ACC3-A9D2-4160-8B01-ED5E40C7E189}</author>
+    <author>tc={5A482186-F8B0-4721-BAB6-AA12B84DC195}</author>
+    <author>tc={5489723F-98BE-48A3-9BEE-41627AB309AB}</author>
+    <author>tc={24497671-CD24-42BA-A892-1D9B4829AD51}</author>
+    <author>tc={4000C2C9-1249-4C51-ABEA-466F92E1810B}</author>
+    <author>tc={E98452AD-1B41-492A-B6A6-FF2BFA437ADE}</author>
+    <author>tc={A89E9DD6-6233-400D-A1D8-3EA3584E1725}</author>
+    <author>tc={1DD4B513-0EC7-472B-AA76-F7140FE48B4E}</author>
+    <author>tc={B32CBE22-EA4E-4B50-9220-DFCBAD24D24C}</author>
+    <author>tc={1AE28864-5635-48BA-A24C-742FBA5CB0F2}</author>
+    <author>tc={C02CFA98-42BE-4FB7-88D5-81435EDA7417}</author>
+    <author>tc={67C72576-4EBB-4155-8BBD-0EFDB0C573B9}</author>
+    <author>tc={C8BA079A-770E-4D28-A0A8-7EC7E1AE781E}</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{B9A5ACC3-A9D2-4160-8B01-ED5E40C7E189}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Change observe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="1" shapeId="0" xr:uid="{5A482186-F8B0-4721-BAB6-AA12B84DC195}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Switch step 3 and 4 results</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="2" shapeId="0" xr:uid="{5489723F-98BE-48A3-9BEE-41627AB309AB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    what is i_rs_vector 0x07 supposed to be?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="3" shapeId="0" xr:uid="{24497671-CD24-42BA-A892-1D9B4829AD51}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Change 0x07</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="4" shapeId="0" xr:uid="{4000C2C9-1249-4C51-ABEA-466F92E1810B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Observe is spelled wrong</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="5" shapeId="0" xr:uid="{E98452AD-1B41-492A-B6A6-FF2BFA437ADE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Observe spelled wrong</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="6" shapeId="0" xr:uid="{A89E9DD6-6233-400D-A1D8-3EA3584E1725}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Observe spelled wrong
+Reply:
+    You set i_reset to 0 two times here</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="7" shapeId="0" xr:uid="{1DD4B513-0EC7-472B-AA76-F7140FE48B4E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    observe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="8" shapeId="0" xr:uid="{B32CBE22-EA4E-4B50-9220-DFCBAD24D24C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    observe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="9" shapeId="0" xr:uid="{1AE28864-5635-48BA-A24C-742FBA5CB0F2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    4. needs to be written as 0x00040_0000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="10" shapeId="0" xr:uid="{C02CFA98-42BE-4FB7-88D5-81435EDA7417}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Observe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="11" shapeId="0" xr:uid="{67C72576-4EBB-4155-8BBD-0EFDB0C573B9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    4. 0x0040_0000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="12" shapeId="0" xr:uid="{C8BA079A-770E-4D28-A0A8-7EC7E1AE781E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="等线"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    you don't specify that i_Reset was ever 1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="374">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -70,15 +315,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CONFIG_REG_TC_01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>‘o_reg_ack’ outputs 1 for one 
-clock cycle when any bit within ‘i_rs_vector[30:0]’ is set to 1 for the previous clock cycle, else ‘o_reg_ack’ is set to 0.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_02</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -91,73 +327,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1.  'i_r_neg_w' = 0
-'i_rs_vector[30:0]' = 0x0000_0001
-'i_reg_w_bus[31:0]' = 0xffff_ffff
-2.'i_rs_vector[30:0]' = 0x0000_0000
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Step2:
- 'o_reg_error' = 0
-Step3:
- 'o_reg_error' = 1 
-Step4:
- 'o_reg_error' = 0
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_r_neg_w' to 0
-, 'i_rs_vector[30:0]' to 0x0000_0001 and 'i_reg_w_bus[31:0]' to 0xffff_ffff on first rising edge of 'i_sys_clk' for this test case
-2.Set 'i_rs_vector[30:0]' to 0x0000_0000 and observe 'o_reg_error' on second rising edge of 'i_sys_clk' for this test case.
-3. Observe  'o_reg_error' on third rising edge of 'i_sys_clk' for this test case.
-4. Observe  'o_reg_error' on fourth rising edge of 'i_sys_clk' for this test case.
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CONFIG_REG_TC_03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>‘o_interrupt’ outputs 1 
-when any of the bits in the internal interrupt status register is set to 1 while the corresponding bit positions in the internal interrupt enable register bits are set to 1, else ‘o_interrupt’ is set to 0.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' to 0, 'i_rs_vector' to 0x07 'i_reg_w_bus[31:0]' =0x00, 'i_r_neg_w'=0 and 'i_sleep' = 1 on the 1st rising edge of 'i_sys_clk' for this test case
-2 Observe 'o_interrupt' on the 3rd  rising egde of 'i_sys_clk' for this test case.
-3.Set 'i_reset' to 0, 'i_rs_vector' to 0x07 'i_reg_w_bus[31:0]' =0x0020_0000, 'i_r_neg_w'=0  on the 4th rising edge of 'i_sys_clk' for this test case
-4.Observe 'o_interrupt' on the 6th rising egde of 'i_sys_clk' for this test case.
-5. Set 'i_sleep' = 0 ont the 7th rirsing edge of 'i_sys_clk' for this test case
-6.Observe 'o_interrupt' on the 9th rising egde of 'i_sys_clk' for this test case.
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. 'i_reset' = 0
- 'i_rs_vector' = 0x07
- 'i_reg_w_bus[31:0]' =0x00,
- 'i_r_neg_w'=0 
- 'i_sleep' = 1 
-3.'i_reg_w_bus[31:0]' =0x0020_0000
-5.'i_sleep' = 0
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step 2: 
-'o_interrupt'  = 0
-Step 4: 
-'o_interrupt'  = 1
-Step 6: 
-'o_interrupt'  = 0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -172,31 +342,6 @@
     <t>‘o_soft_reset’ is set to 1 for one
 clock cycle when ‘i_sys_clk
 ’ transitions from 0 to 1 while bit 31 of i_reg_w_bus is set to 1 and i_rs_vector bit 0 is set to 1, else ‘o_soft_reset’ is set to 0.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. Set 'i_reset' to 0, 'i_rs_vector' to 0x01 
-'i_reg_w_bus[31:0]' =0x2000_0000, 'i_r_neg_w'=0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector' = 0x00 on the 2rd rising edge of 'i_sys_clk' for this test case
-3.Observe 'o_soft_reset' on the 3rd  rising egde of 'i_sys_clk' for this test case.
-4 Observe 'o_soft_reset' on the 4th  rising egde of 'i_sys_clk' for this test case.
-5. Set 'i_reg_w_bus[31:0]' =0x0000_0000
-and 'i_rs_vector' = 0x01  on the 5th rising edge of 'i_sys_clk' for this test case
-6. Set 'i_rs_vector' = 0x00 on the 6th rising edge of 'i_sys_clk' for this test case
-7. observe 'o_soft_reset' on the 7th rising edge of 'i_sys_clk' for this test case
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.'i_reset' = 0
- 'i_rs_vector' = 0x01
- 'i_reg_w_bus[31:0]' =0x2000_0000,
- 'i_r_neg_w'=0 
-2. 'i_rs_vector' = 0x00
-5. 'i_rs_vector' = 0x01
- 'i_reg_w_bus[31:0]' =0x0000_0000,
-6. 'i_rs_vector' = 0x00</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -218,16 +363,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> ‘o_tx_fifo_data[127:0]’  outputs
- the data that is stored in the four internal registers from most significant bit to least significant bit in this corresponding order: tx ID[31:0], tx DLC[31:0], tx DW1[31:0], and tx DW2[31:0].</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stpp 9: 
-'o_tx_fifo_data[127:0]' = 0000_0001_0000_0001_0000_0001_0000_0000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_06</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -238,24 +373,6 @@
   <si>
     <t xml:space="preserve"> ‘o_tx_w_en’ is set to 1
  for one clock cycle when ‘i_sys_clk’ transition from 0 to 1 while i_tx_full is 0 and i_rs_vector[13] was set to 1 in the previous clock cycle, else ‘o_tx_w_en’ is set to 0.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset' = 0
- 'i_rs_vector[30:0]' = 0x0000_0400
- 'i_reg_w_bus[31:0]' =0x0000_0001,
- 'i_r_neg_w'=0 
-2. 'i_rs_vector[30:0]' = 0x0000_0000
-3.'i_rs_vector[30:0]' = 0x0000_0800
- 'i_reg_w_bus[31:0]' =0x0000_0001,
-4.'i_rs_vector[30:0]' = 0x0000_0000
-5.'i_rs_vector[30:0]' = 0x0000_1000
- 'i_reg_w_bus[31:0]' =0x0000_0001,
-6.'i_rs_vector[30:0]' = 0x0000_0000
-7.'i_rs_vector[30:0]' = 0x0000_2000
- 'i_reg_w_bus[31:0]' =0x0000_0000,
-8..'i_rs_vector[30:0]' = 0x0000_0000
-</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -276,33 +393,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> ‘o_hpb_data[127:0]’ outputs the data that is stored in the four internal registers from most  significant bit to least significant bit in this corresponding order: hpb ID[31:0], hpb DLC[31:0], hpb DW1[31:0], and hpb DW2[31:0].</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset' = 0
- 'i_rs_vector[30:0]' = 0x0000_4000
- 'i_reg_w_bus[31:0]' =0x0000_0001,
- 'i_r_neg_w'=0 
-2. 'i_rs_vector[30:0]' = 0x0000_0000
-3.'i_rs_vector[30:0]' = 0x0000_8000
- 'i_reg_w_bus[31:0]' =0x0000_0001,
-4.'i_rs_vector[30:0]' = 0x0000_0000
-5.'i_rs_vector[30:0]' = 0x0001_0000
- 'i_reg_w_bus[31:0]' =0x0000_0001,
-6.'i_rs_vector[30:0]' = 0x0000_0000
-7.'i_rs_vector[30:0]' = 0x0002_0000
- 'i_reg_w_bus[31:0]' =0x0000_0000,
-8..'i_rs_vector[30:0]' = 0x0000_0000
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stpp 9: 
-'o_hpb_data[127:0]' = 0000_0001_0000_0001_0000_0001_0000_0000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_08</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -316,32 +406,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Step3.
-'o_heb_r_en' = 1
-Step4
-'o_heb_r_en' = 0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_09</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CONFIG_REG_TC_09</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> ‘o_hpb_full’ is to 1 for one clock cycle when ‘i_sys_clk’ transitions from 0 to 1 while i_r_neg_w is 0 and i_rs_vector is 0x20000 in the previous clock cycle, else o_hpb_full is 0.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 3:
-'o_hpb_full' = 1
-Step 4:
-'o_hpb_full' = 0
-Step 6:
-'o_hpb_full' = 0
-</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -690,12 +759,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1.'i_reset' =0 , 'i_rx_fifo_data[31:0]'=0000_0001_0000_0001_0000_0001_0000_0000,
-'o_rx_r_en' =1
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3
 rx_ID[31:0] = 0x0000_0001</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -714,18 +777,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. Set 'i_reset' =0 , 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
-2. wait for one clock cyle
-3. Observe value of rx_DLC[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Set 'i_reset' =0 , 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
-2. wait for one clock cyle
-3. Observe value of rx_ID[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3
 rx_DLC[31:0] = 0x0000_0001</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -739,12 +790,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. Set 'i_reset' =0 , 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
-2. wait for one clock cyle
-3. Observe value of rx_DW1[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3
 rx_DW1[31:0] = 0x0000_0001</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -758,12 +803,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1. Set 'i_reset' =0 , 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
-2. wait for one clock cyle
-3. Observe value of rx_DW2[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3
 rx_DW1[31:0] = 0x0000_0000</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -779,13 +818,6 @@
   <si>
     <t>Bit position 27 in the internal error status register store
  the value input into i_acker every clock cycle synched to i_sys_clk.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.  'i_reset' =0
- 'i_acker'=1
-2. 'i_reset' =0
- 'i_acker'=0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -796,13 +828,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_acker'=1 on the rising edge of 'i_can_clk'
-2. Observe internal error status register ISE[27] on next rising edge of 'i_sys_clk' 
-3. Set 'i_reset' =0, 'i_acker'=0 on the rising edge of 'i_can_clk'
-4 Observe internal error status register ISE[27] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_33</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -813,20 +838,6 @@
   <si>
     <t>Bit position 28 in the internal error status register store
  the value input into i_berr every clock cycle synched to i_sys_clk.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_berr'=1 on the rising edge of 'i_can_clk'
-2. Observe internal error status register ISE[28] on next rising edge of 'i_sys_clk' 
-3. Set 'i_reset' =0, 'i_berr'=0 on the rising edge of 'i_can_clk'
-4 Observe internal error status register ISE[28] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.  'i_reset' =0
- 'i_berr'=1
-2. 'i_reset' =0
- 'i_berr'=0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -865,22 +876,8 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1.  'i_reset' =0
- 'i_ster'=1
-2. 'i_reset' =0
- 'i_ster'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Bit position 30 in the internal error status register store
  the value input into i_fmer every clock cycle synched to i_sys_clk.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.  'i_reset' =0
- 'i_fmer'=1
-2. 'i_reset' =0
- 'i_fmer'=0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -904,27 +901,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_fmer'=1 on the rising edge of 'i_can_clk'
-2. Observe internal error status register ISE[30] on next rising edge of 'i_sys_clk' 
-3. Set 'i_reset' =0, 'i_fmer'=0 on the rising edge of 'i_can_clk'
-4 Observe internal error status register ISE[30] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_ster'=1 on the rising edge of 'i_can_clk'
-2. Observe internal error status register ISE[29] on next rising edge of 'i_sys_clk' 
-3. Set 'i_reset' =0, 'i_ster'=0 on the rising edge of 'i_can_clk'
-4 Observe internal error status register ISE[29] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_crcer'=1 on the rising edge of 'i_can_clk'
-2. Observe internal error status register ISE[31] on next rising edge of 'i_sys_clk' 
-3. Set 'i_reset' =0, 'i_crcer'=0 on the rising edge of 'i_can_clk'
-4 Observe internal error status register ISE[31] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1.  'i_reset' =0
  'i_crer'=1
 2. 'i_reset' =0
@@ -951,13 +927,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1'i_reset' =0,
- 'i_acfbsy'=1
-4'i_reset' =0,
- 'i_acfbsy'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_REG_38</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -967,15 +936,6 @@
   </si>
   <si>
     <t>Bit position [24:23] in the internal status register stores the value input into ‘i_estat’[1:0] every clock cycle synched to i_sys_clk.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_acfbsy'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle
-3. Observe internal status register ISR[20] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_acfbsy'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle
-6.Observe internal status register ISR[20] on next rising edge of 'i_sys_clk' </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -986,22 +946,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_estat'[1:0]=11 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[24:23] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_estat'[1:0]=00 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[24:23] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_estat'[1:0]=11
-4'i_reset' =0,
- 'i_estat'[1:0]=00</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[24:23]=1 
 Step 6:
@@ -1036,39 +980,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_errwrn'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[25] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_errwrn'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[25] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Bit position 26 in the internal status register stores the value input into ‘i_bbsy’ every clock cycle synched to i_sys_clk.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_bbsy'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[26] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_bbsy'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[26] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_errwrn=1
-4'i_reset' =0,
- 'i_errwen'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_bbsy=1
-4'i_reset' =0,
- 'i_bbsy'=0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1091,22 +1003,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_bidle'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[27] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_bidle'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[27] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_bidle=1
-4'i_reset' =0,
- 'i_bidle'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[27]=1 
 Step 6:
@@ -1126,22 +1022,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_normal'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[28] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_normal'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[28] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_normal=1
-4'i_reset' =0,
- 'i_normal'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[28]=1 
 Step 6:
@@ -1161,22 +1041,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_sleep'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[29] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_sleep'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[29] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_sleep=1
-4'i_reset' =0,
- 'i_sleep'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[29]=1 
 Step 6:
@@ -1196,22 +1060,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_lback'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[30] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_lback'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[30] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_lback=1
-4'i_reset' =0,
- 'i_lback'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[30]=1 
 Step 6:
@@ -1231,22 +1079,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_config'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[31] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_config'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[31] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_config=1
-4'i_reset' =0,
- 'i_config'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[31]=1 
 Step 6:
@@ -1266,22 +1098,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_wakeup'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[20] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_wakeup'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[20] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_wakeup=1
-4'i_reset' =0,
- 'i_wakeup'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[20]=1 
 Step 6:
@@ -1301,15 +1117,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_sleep'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[21] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_sleep'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[21] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[21]=1 
 Step 6:
@@ -1329,22 +1136,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_bsoff'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[22] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_bsoff'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[22] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_bsoff=1
-4'i_reset' =0,
- 'i_bsoff'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[22]=1 
 Step 6:
@@ -1364,22 +1155,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_error'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[23] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_error'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[23] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_error=1
-4'i_reset' =0,
- 'i_error'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[23]=1 
 Step 6:
@@ -1399,22 +1174,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_rxnemp'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[24] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_rxnemp'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[24] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_rxnemp=1
-4'i_reset' =0,
- 'i_rxnemp'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[24]=1 
 Step 6:
@@ -1434,22 +1193,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_rxoflw'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[25] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_rxoflw'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[25] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_rxoflw=1
-4'i_reset' =0,
- 'i_rxoflw'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[25]=1 
 Step 6:
@@ -1469,22 +1212,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_rxuflw'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[26] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_rxuflw'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[26] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_rxuflw=1
-4'i_reset' =0,
- 'i_rxuflw'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[26]=1 
 Step 6:
@@ -1504,22 +1231,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_rxok'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[27] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_rxok'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[27] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_rxok=1
-4'i_reset' =0,
- 'i_rxok'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[27]=1 
 Step 6:
@@ -1535,22 +1246,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'o_hpb_full'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[28] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'o_hpb_full'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[28] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'o_hpb_full=1
-4'i_reset' =0,
- 'o_hpb_full'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[28]=1 
 Step 6:
@@ -1574,22 +1269,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_tx_full'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[29] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_tx_full'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[29] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_tx_full=1
-4'i_reset' =0,
- 'i_tx_full'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[29]=1 
 Step 6:
@@ -1609,13 +1288,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1'i_reset' =0,
- 'i_txok=1
-4'i_reset' =0,
- 'i_txok'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[30]=1 
 Step 6:
@@ -1636,31 +1308,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_arblst'=1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_arblst'=0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_txok'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_txok'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_arblst=1
-4'i_reset' =0,
- 'i_arblst'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IISR[31]=1 
 Step 6:
@@ -1680,22 +1327,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_rec'[7:0]=0x1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt error count register IIECR[23:16] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0,'i_rec'[7:0]=0x0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt error count register IIECR[23:16] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
-'i_rec'[7:0]=0x1
-4'i_reset' =0,
-'i_rec'[7:0]=0x0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IIECR[23:16]=0x1
 Step 6:
@@ -1715,22 +1346,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_tec'[7:0]=0x1 on the rising edge of 'i_can_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal interrupt error count register IIECR[31:24] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0,'i_tec'[7:0]=0x0 on the rising edge of 'i_can_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal interrupt error count register IIECR[31:24] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
-'i_tec'[7:0]=0x1
-4'i_reset' =0,
-'i_tec'[7:0]=0x0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 IIECR[31:24]=0x1
 Step 6:
@@ -1751,27 +1366,92 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset' =0, 'i_tx_full'=1 on the rising edge of 'i_sys_clk'
-2.wait for one clock cycle of ' i_sys_clk'
-3. Observe internal status register ISR[21] on next rising edge of 'i_sys_clk' 
-4. Set 'i_reset' =0, 'i_tx_full'=0 on the rising edge of 'i_sys_clk'
-5, wait for one clock cycle of ' i_sys_clk'
-6.Observe internal status register ISR[21] on next rising edge of 'i_sys_clk' </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1'i_reset' =0,
- 'i_tx_full'=1 
-4'i_reset' =0,
- 'i_tx_full'=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 3:
 ISR[21]=1 
 Step 6:
 ISR[21] =0</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. i_rs_vector[30:0] = 0x0000_0001
+2. i_rs_vector[30:0] = 0x0000_0000
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x0800_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x1000_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x2000_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x4000_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x0080_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x0100_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x0200_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_reset = 1 
+2.  'i_reset = 0' 
+    'i_rs_vector[30:0]' = 0x0400_0000 ,
+   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
+3.'i_rs_vector[30:0]' = 0x0000_000 ,
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The internal register,
+ rx DLC[31:0], stores the value,‘i_rx_fifo_data[95:64]’, when ‘o_rx_r_en’ is 1 and ‘i_sys_clk’ transitions from 0 to 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The internal register,
+ rx DW1[31:0], stores the value,‘i_rx_fifo_data[63:32]’, when ‘o_rx_r_en’ is 1 and ‘i_sys_clk’ transitions from 0 to 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The internal register,
+ rx DW2[31:0], stores the value,‘i_rx_fifo_data[31:0]’, when ‘o_rx_r_en’ is 1 and ‘i_sys_clk’ transitions from 0 to 1.</t>
   </si>
   <si>
     <t>At step 18:
@@ -1795,201 +1475,732 @@
 o_afmr1,2,3,4=0x0000_0001
 o_afir1,2,3,4=0x0000_0001
 o_uaf1,2,3,4=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONFIG_REG_TC_01</t>
+  </si>
+  <si>
+    <t>‘o_reg_ack’ outputs 1 for one 
+clock cycle when any bit within ‘i_rs_vector[30:0]’ is set to 1 for the previous clock cycle, else ‘o_reg_ack’ is set to 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_r_neg_w' to 0
+, 'i_rs_vector[30:0]' to 0x0000_0001 and 'i_reg_w_bus[31:0]' to 0xffff_ffff on first rising edge of 'i_sys_clk' for this test case
+2.Set 'i_rs_vector[30:0]' to 0x0000_0000 and observe 'o_reg_error' on second rising edge of 'i_sys_clk' for this test case.
+3. Observe  'o_reg_error' on third rising edge of 'i_sys_clk' for this test case.
+4. Observe  'o_reg_error' on fourth rising edge of 'i_sys_clk' for this test case.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  'i_r_neg_w' = 0
+'i_rs_vector[30:0]' = 0x0000_0001
+'i_reg_w_bus[31:0]' = 0xffff_ffff
+2.'i_rs_vector[30:0]' = 0x0000_0000
+</t>
+  </si>
+  <si>
+    <t>CONFIG_REG_TC_03</t>
+  </si>
+  <si>
+    <t>‘o_interrupt’ outputs 1 
+when any of the bits in the internal interrupt status register is set to 1 while the corresponding bit positions in the internal interrupt enable register bits are set to 1, else ‘o_interrupt’ is set to 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ‘o_tx_fifo_data[127:0]’  outputs
+ the data that is stored in the four internal registers from most significant bit to least significant bit in this corresponding order: tx ID[31:0], tx DLC[31:0], tx DW1[31:0], and tx DW2[31:0].</t>
+  </si>
+  <si>
+    <t>Stpp 9: 
+'o_tx_fifo_data[127:0]' = 0000_0001_0000_0001_0000_0001_0000_0000</t>
+  </si>
+  <si>
+    <t>Stpp 9: 
+'o_hpb_data[127:0]' = 0000_0001_0000_0001_0000_0001_0000_0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ‘o_hpb_data[127:0]’ outputs the data that is stored in the four internal registers from most  significant bit to least significant bit in this corresponding order: hpb ID[31:0], hpb DLC[31:0], hpb DW1[31:0], and hpb DW2[31:0].</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ‘o_hpb_full’ is to 1 for one clock cycle when ‘i_sys_clk’ transitions from 0 to 1 while i_r_neg_w is 0 and i_rs_vector is 0x20000 in the previous clock cycle, else o_hpb_full is 0.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Set 'i_rs_vector[30:0]' to 0x0000_0001 on the first rising edge of 'i_sys_clk' for this test case
 2.Set 'i_rs_vector[30:0]' to 0x0000_0000 on the second rising edge of 'i_sys_clk' for this test case
-3.Oberve 'o_reg_ack' on third rising edge of 'i_sys_clk' for this test case
-4.Oberve 'o_reg_ack' on fourth rising edge of 'i_sys_clk' for this test case
+3.Observe 'o_reg_ack' on third rising edge of 'i_sys_clk' for this test case
+4.Observe 'o_reg_ack' on fourth rising edge of 'i_sys_clk' for this test case
 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0800_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afmr1' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x1000_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afmr2' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x2000_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afmr3' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x4000_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afmr4' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0080_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afir1' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0100_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afir2' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0200_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afir3' on the 4th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0400_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
+4 Observe 'o_afir4' on the 4th rising edge of 'i_sys_clk' for this test case</t>
   </si>
   <si>
     <t xml:space="preserve">
 Step 3:
-'o_reg_ack' = 1
+'o_reg_ack' = 0
 Step 4:
-'o_reg_ack' = 0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0400 ,'i_reg_w_bus[31:0]' =0x0000_0001, 'i_r_neg_w'=0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_rs_vector{30:0]' to 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Set 'i_rs_vector[30:0]' = 0x0000_0800 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 3rd rising edge of 'i_sys_clk' for this test case
-4. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set 'i_rs_vector[30:0]' = 0x0000_1000 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 5th rising edge of 'i_sys_clk' for this test case
-6. Set 'i_rs_vector' to 0x0000_0000 on the 6th rising edge of 'i_sys_clk' for this test case
-7. Set 'i_rs_vector[30:0]' = 0x0000_2000 ,'i_reg_w_bus[31:0]' =0x0000_0000, on the 7th rising edge of 'i_sys_clk' for this test case
-8. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 8th rising edge of 'i_sys_clk' for this test case
-9. Observe 'o_tx_fifo_data[127:0] on the 9th rising edge of 'i_sys_clk' for this test case
+'o_reg_ack' = 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Step2:
+ 'o_reg_error' = 0
+Step3:
+ 'o_reg_error' = 0
+Step4:
+ 'o_reg_error' = 1
 </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_2000 ,'i_tx_full'=0 on the 1st rising edge of 'i_sys_clk' for this test case
-2.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Observe 'o_tx_w_en' on the 3rd tising edge of 'i_sys_clk' for this test case.
-4. 'i_rs_vector[30:0]' = 0x0000_2000 ,'i_tx_full'=1 on the 4th rising edge of 'i_sys_clk' for this test case
-5.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 5th rising edge of 'i_sys_clk' for this test case
-6.Observe 'o_tx_w_en' on the 6th tising edge of 'i_sys_clk' for this test case.
-7.'i_rs_vector[30:0]' = 0x0000_0000 ,'i_tx_full'=0 on the 7th rising edge of 'i_sys_clk' for this test case
-8.Observe 'o_tx_w_en' on the 9th tising edge of 'i_sys_clk' for this test case.
+    <t xml:space="preserve">1.
+ 'i_rs_vector' = 0x07
+ 'i_reg_w_bus[31:0]' =0x00,
+ 'i_r_neg_w'=0 
+ 'i_sleep' = 1 
+3.'i_reg_w_bus[31:0]' =0x0020_0000
+5.'i_sleep' = 0
 </t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_2000 
-  'i_tx_full'=0 
-2.'i_rs_vector[30:0]' = 0x0000_0000 
-4,'i_rs_vector[30:0]' = 0x0000_2000 
-'i_tx_full'=1 
-5.'i_rs_vector[30:0]' = 0x0000_0000 
-7.'i_rs_vector[30:0]' = 0x0000_0000 
-'i_tx_full'=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0400 ,'i_reg_w_bus[31:0]' =0x0000_0001, 'i_r_neg_w'=0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_rs_vector{30:0]' to 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Set 'i_rs_vector[30:0]' = 0x0000_0800 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 3rd rising edge of 'i_sys_clk' for this test case
-4. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set 'i_rs_vector[30:0]' = 0x0001_0000 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 5th rising edge of 'i_sys_clk' for this test case
-6. Set 'i_rs_vector' to 0x0000_0000 on the 6th rising edge of 'i_sys_clk' for this test case
-7. Set 'i_rs_vector[30:0]' = 0x0002_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000, on the 7th rising edge of 'i_sys_clk' for this test case
-8. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 8th rising edge of 'i_sys_clk' for this test case
-9. Observe 'o_hpb_data[127:0] on the 9th rising edge of 'i_sys_clk' for this test case
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector' to 0x07 'i_reg_w_bus[31:0]' =0x00, 'i_r_neg_w'=0 and 'i_sleep' = 1 on the 1st rising edge of 'i_sys_clk' for this test case
+2 Observe 'o_interrupt' on the 4th  rising egde of 'i_sys_clk' for this test case.
+3.Set  'i_rs_vector' to 0x80 'i_reg_w_bus[31:0]' =0x0020_0000, 'i_r_neg_w'=0  on the 5th rising edge of 'i_sys_clk' for this test case
+4.Observe 'o_interrupt' on the 9th rising egde of 'i_sys_clk' for this test case.
+5. Set 'i_sleep' = 0 ont the 10th rirsing edge of 'i_sys_clk' for this test case
+6.Observe 'o_interrupt' on the 13th rising egde of 'i_sys_clk' for this test case.
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0002_0000 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3,Observe 'o_hpb_r_en' on the 3rd rising edge of 'i_sys_clk' for this test case
-4,Observe 'o_hpb_r_en' on the 4th rising edge of 'i_sys_clk' for this test case
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 2: 
+'o_interrupt'  = 0
+Step 4: 
+'o_interrupt'  = 1
+Step 6: 
+'o_interrupt'  = 0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step3.
+'o_heb_r_en' = 0
+Step4
+'o_heb_r_en' = 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 3:
+'o_hpb_full' = 0
+Step 4:
+'o_hpb_full' = 1
+Step 6:
+'o_hpb_full' = 0
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0002_0000 
-2. 'i_rs_vector[30:0]' = 0x0000_0000 </t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0002_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2.Set 'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Observe 'o_hpb_full' on the 3rd rising edge of 'i_sys_clk' for this test case
-4.Observe 'o_hpb_full' on the 4th rising edge of 'i_sys_clk' for this test case
-5.Set 'i_rs_vector[30:0]' = 0x0002_0000 and 'i_r_neg_w'  = 1 on the 5th rising edge of 'i_sys_clk' for this test case
-6.Observe 'o_hpb_full' on the 7th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1.'i_reset = 0',
- 'i_rs_vector[30:0]' = 0x0002_0000
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x4000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_uaf2' on the 3rd rising edge of 'i_sys_clk' for this test case
+4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6 Observe 'o_uaf2' on the 6th rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x2000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_uaf3' on the 3rd rising edge of 'i_sys_clk' for this test case
+4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6 Observe 'o_uaf3' on the 6th rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 
+ 'i_rs_vector[30:0]' = 0x0040_0000
+ 'i_reg_w_bus[31:0]' =0x1000_0000
  'i_r_neg_w' = 0
-2. 'i_rs_vector[30:0]' = 0x0000_0000
-5. 'i_rs_vector[30:0]' = 0x0002_0000
- 'i_r_neg_w' = 1</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x4000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_lback' on the 3rd rising edge of 'i_can_clk' for this test case
-4. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6. Oberve 'o_lback' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0002 
+2.'i_rs_vector[30:0]' = 0x0000_0000
+4. 'i_rs_vector[30:0]' = 0x0004_0000 
+ 'i_reg_w_bus[31:0]' =0x0000_0000
+ 'i_r_neg_w' = 0
+5.'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 
+ 'i_rs_vector[30:0]' = 0x0040_0000
+ 'i_reg_w_bus[31:0]' =0x2000_0000
+ 'i_r_neg_w' = 0
+2.'i_rs_vector[30:0]' = 0x0000_0000
+4. 'i_rs_vector[30:0]' = 0x0004_0000 
+ 'i_reg_w_bus[31:0]' =0x0000_0000
+ 'i_r_neg_w' = 0
+5.'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set  'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
+2. wait for one clock cyle
+3. Observe value of rx_ID[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  'i_rx_fifo_data[31:0]'=0000_0001_0000_0001_0000_0001_0000_0000,
+'o_rx_r_en' =1
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Se 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
+2. wait for one clock cyle
+3. Observe value of rx_DLC[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. , 'i_rx_fifo_data[31:0]'=0000_0001_0000_0001_0000_0001_0000_0000,
+'o_rx_r_en' =1
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  'i_ster'=1 on the rising edge of 'i_can_clk'
+2. Observe internal error status register ISE[29] on next rising edge of 'i_sys_clk' 
+3. , 'i_ster'=0 on the rising edge of 'i_can_clk'
+4 Observe internal error status register ISE[29] on next rising edge of 'i_sys_clk' </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  
+ 'i_ster'=1
+2. 
+ 'i_ster'=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set , 'i_fmer'=1 on the rising edge of 'i_can_clk'
+2. Observe internal error status register ISE[30] on next rising edge of 'i_sys_clk' 
+3. Set , 'i_fmer'=0 on the rising edge of 'i_can_clk'
+4 Observe internal error status register ISE[30] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1.  
+ 'i_fmer'=1
+2. 
+ 'i_fmer'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_crcer'=1 on the rising edge of 'i_can_clk'
+2. Observe internal error status register ISE[31] on next rising edge of 'i_sys_clk' 
+3. Set  'i_crcer'=0 on the rising edge of 'i_can_clk'
+4 Observe internal error status register ISE[31] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_acfbsy'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle
+3. Observe internal status register ISR[20] on next rising edge of 'i_sys_clk' 
+4. Set  'i_acfbsy'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle
+6.Observe internal status register ISR[20] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_acfbsy'=1
+4
+ 'i_acfbsy'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_estat'[1:0]=11 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[24:23] on next rising edge of 'i_sys_clk' 
+4. Set  'i_estat'[1:0]=00 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[24:23] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_estat'[1:0]=11
+4
+ 'i_estat'[1:0]=00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_errwrn'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[25] on next rising edge of 'i_sys_clk' 
+4. Set  'i_errwrn'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[25] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_errwrn=1
+4
+ 'i_errwen'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_bbsy'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[26] on next rising edge of 'i_sys_clk' 
+4. Set  'i_bbsy'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[26] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_bbsy=1
+4
+ 'i_bbsy'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_bidle'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[27] on next rising edge of 'i_sys_clk' 
+4. Set  'i_bidle'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[27] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_bidle=1
+4
+ 'i_bidle'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_normal'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[28] on next rising edge of 'i_sys_clk' 
+4. Set  'i_normal'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[28] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_normal=1
+4
+ 'i_normal'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_sleep'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[29] on next rising edge of 'i_sys_clk' 
+4. Set  'i_sleep'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[29] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_sleep=1
+4
+ 'i_sleep'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_lback'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[30] on next rising edge of 'i_sys_clk' 
+4. Set  'i_lback'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[30] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_lback=1
+4
+ 'i_lback'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_config'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[31] on next rising edge of 'i_sys_clk' 
+4. Set  'i_config'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[31] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_config=1
+4
+ 'i_config'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_wakeup'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[20] on next rising edge of 'i_sys_clk' 
+4. Set  'i_wakeup'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[20] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_wakeup=1
+4
+ 'i_wakeup'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_sleep'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[21] on next rising edge of 'i_sys_clk' 
+4. Set  'i_sleep'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[21] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_bsoff'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[22] on next rising edge of 'i_sys_clk' 
+4. Set  'i_bsoff'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[22] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_bsoff=1
+4
+ 'i_bsoff'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_error'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[23] on next rising edge of 'i_sys_clk' 
+4. Set  'i_error'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[23] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_error=1
+4
+ 'i_error'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_rxnemp'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[24] on next rising edge of 'i_sys_clk' 
+4. Set  'i_rxnemp'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[24] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_rxnemp=1
+4
+ 'i_rxnemp'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_rxoflw'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[25] on next rising edge of 'i_sys_clk' 
+4. Set  'i_rxoflw'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[25] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_rxoflw=1
+4
+ 'i_rxoflw'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_rxuflw'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[26] on next rising edge of 'i_sys_clk' 
+4. Set  'i_rxuflw'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[26] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_rxuflw=1
+4
+ 'i_rxuflw'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_rxok'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[27] on next rising edge of 'i_sys_clk' 
+4. Set  'i_rxok'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[27] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_rxok=1
+4
+ 'i_rxok'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'o_hpb_full'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[28] on next rising edge of 'i_sys_clk' 
+4. Set  'o_hpb_full'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[28] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'o_hpb_full=1
+4
+ 'o_hpb_full'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_tx_full'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[29] on next rising edge of 'i_sys_clk' 
+4. Set  'i_tx_full'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[29] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_tx_full=1
+4
+ 'i_tx_full'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_txok'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' 
+4. Set  'i_txok'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_txok=1
+4
+ 'i_txok'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_arblst'=1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' 
+4. Set  'i_arblst'=0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt status register IISR[30] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_arblst=1
+4
+ 'i_arblst'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_rec'[7:0]=0x1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt error count register IIECR[23:16] on next rising edge of 'i_sys_clk' 
+4. Set 'i_rec'[7:0]=0x0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt error count register IIECR[23:16] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+'i_rec'[7:0]=0x1
+4
+'i_rec'[7:0]=0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_tec'[7:0]=0x1 on the rising edge of 'i_can_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal interrupt error count register IIECR[31:24] on next rising edge of 'i_sys_clk' 
+4. Set 'i_tec'[7:0]=0x0 on the rising edge of 'i_can_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal interrupt error count register IIECR[31:24] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+'i_tec'[7:0]=0x1
+4
+'i_tec'[7:0]=0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_tx_full'=1 on the rising edge of 'i_sys_clk'
+2.wait for one clock cycle of ' i_sys_clk'
+3. Observe internal status register ISR[21] on next rising edge of 'i_sys_clk' 
+4. Set  'i_tx_full'=0 on the rising edge of 'i_sys_clk'
+5, wait for one clock cycle of ' i_sys_clk'
+6.Observe internal status register ISR[21] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1
+ 'i_tx_full'=1 
+4
+ 'i_tx_full'=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_acker'=1 on the rising edge of 'i_can_clk'
+2. Observe internal error status register ISE[27] on next rising edge of 'i_sys_clk' 
+3. Set  'i_acker'=0 on the rising edge of 'i_can_clk'
+4 Observe internal error status register ISE[27] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_berr'=1 on the rising edge of 'i_can_clk'
+2. Observe internal error status register ISE[28] on next rising edge of 'i_sys_clk' 
+3. Set  'i_berr'=0 on the rising edge of 'i_can_clk'
+4 Observe internal error status register ISE[28] on next rising edge of 'i_sys_clk' </t>
+  </si>
+  <si>
+    <t>1. 
+ 'i_berr'=1
+2.
+ 'i_berr'=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 
+ 'i_acker'=1
+2. 
+ 'i_acker'=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.'i_rx_fifo_data[31:0]'=0000_0001_0000_0001_0000_0001_0000_0000,
+'o_rx_r_en' =1
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
+2. wait for one clock cyle
+3. Observe value of rx_DW2[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 'i_rx_fifo_data[31:0]'=0000_0001_0000_0001_0000_0001_0000_0000,
+'o_rx_r_en' =1
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set 'i_rx_fifo_data[31:0]'=0x0000_0001_0000_0001_0000_0001_0000_0000, and 'o_rx_r_en' =1  on the 1st rising edge of 'i_sys_clk' for this test case
+2. wait for one clock cyle
+3. Observe value of rx_DW1[31:0] on the 3rd rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector[30:0]' = 0x0040_0000
  'i_reg_w_bus[31:0]' =0x4000_0000
  'i_r_neg_w' = 0
 2.'i_rs_vector[30:0]' = 0x0000_0000
-4,'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0002 
+4. 'i_rs_vector[30:0]' = 0x0004_0000 
  'i_reg_w_bus[31:0]' =0x0000_0000
  'i_r_neg_w' = 0
-5,'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x8000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+5.'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x8000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
 2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_sleep' on the 3rd rising edge of 'i_can_clk' for this test case
-4. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6. Oberve 'o_sleep' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0002 
+3. Observe 'o_uaf1' on the 3rd rising edge of 'i_sys_clk' for this test case
+4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6 Observe 'o_uaf1' on the 6th rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 
+ 'i_rs_vector[30:0]' = 0x0040_0000
  'i_reg_w_bus[31:0]' =0x8000_0000
  'i_r_neg_w' = 0
 2.'i_rs_vector[30:0]' = 0x0000_0000
-4,'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0002 
+4. 'i_rs_vector[30:0]' = 0x0004_0000 
  'i_reg_w_bus[31:0]' =0x0000_0000
  'i_r_neg_w' = 0
-5,'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x1800_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_sjw[1:0]' on the 3rd rising edge of 'i_can_clk' for this test case
-4. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6. Oberve 'o_sjw[1:0]' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0004
- 'i_reg_w_bus[31:0]' =0x1800_0000
+5.'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector[30:0]' = 0x0020_0000 
+  'i_tx_emptyl'=0 
+  'i_r_neg_w' = 1
+2.'i_rs_vector[30:0]' = 0x0000_0000 
+4,'i_rs_vector[30:0]' = 0x0020_0000 
+ 'i_tx_emptyl'=1
+5.'i_rs_vector[30:0]' = 0x0000_0000 
+7.'i_rs_vector[30:0]' = 0x0000_0000 
  'i_r_neg_w' = 0
-2.'i_rs_vector[30:0]' = 0x0000_0000
-4,'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0004
- 'i_reg_w_bus[31:0]' =0x0000_0000
- 'i_r_neg_w' = 0
-5,'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0E00_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_ts2[2:0]' on the 3rd rising edge of 'i_can_clk' for this test case
-4. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6. Oberve 'o_ts2[2:0]' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0004
- 'i_reg_w_bus[31:0]' =0x0E00_0000
- 'i_r_neg_w' = 0
-2.'i_rs_vector[30:0]' = 0x0000_0000
-4,'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0004
- 'i_reg_w_bus[31:0]' =0x0000_0000
- 'i_r_neg_w' = 0
-5,'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0xF000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_ts1[3:0]' on the 3rd rising edge of 'i_can_clk' for this test case
-4. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6. Oberve 'o_ts1[3:0]' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0004
- 'i_reg_w_bus[31:0]' =0xF000_0000
- 'i_r_neg_w' = 0
-2.'i_rs_vector[30:0]' = 0x0000_0000
-4,'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0000_0004
- 'i_reg_w_bus[31:0]' =0x0000_0000
- 'i_r_neg_w' = 0
-5,'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0800_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 and 'i_r_neg_w' = 0 on the rising edge of 'i_sys_clk'
+ 'i_tx_emptyl'=1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector[30:0]' = 0x0020_0000 ,'i_tx_empty'= '0' and 'i_r_neg_w' = 1 on the 1st rising edge of 'i_sys_clk' for this test case
+2.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 2nd rising edge of 'i_sys_clk' for this test case
+3.Observe ‘o_rx_r_en’on the 3rd tising edge of 'i_sys_clk' for this test case.
+4. 'i_rs_vector[30:0]' = 0x0020_0000 ,''i_tx_empty'=1 on the 4th rising edge of 'i_sys_clk' for this test case
+5.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 5th rising edge of 'i_sys_clk' for this test case
+6.Observe ‘o_rx_r_en’ on the 6th tising edge of 'i_sys_clk' for this test case.
+7.'i_rs_vector[30:0]' = 0x0000_0000 ,'i_r_neg_w' = 0 on the 7th rising edge of 'i_sys_clk' for this test case
+8.Observe ‘o_rx_r_en’ on the 9th tising edge of 'i_sys_clk' for this test case.
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  'i_rs_vector[30:0]' = 0x0800_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001  'i_r_neg_w' = 0 '
+2. 'i_rs_vector[30:0]' = 0x0000_00000 
+3. 'i_rs_vector[30:0]' = 0x1000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
+4.'i_rs_vector[30:0]' = 0x0000_00000 
+5.'i_rs_vector[30:0]' = 0x2000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 
+6.'i_rs_vector[30:0]' = 0x0000_00000 
+7.'i_rs_vector[30:0]' = 0x4000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 
+8.'i_rs_vector[30:0]' = 0x0000_00000 9.'i_rs_vector[30:0]' = 0x0080_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
+10.'i_rs_vector[30:0]' = 0x0000_00000 
+11.'i_rs_vector[30:0]' = 0x0100_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
+12.'i_rs_vector[30:0]' = 0x0000_00000 
+13.'i_rs_vector[30:0]' = 0x0200_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 
+15.'i_rs_vector[30:0]' = 0x0000_00000
+16.'i_rs_vector[30:0]' = 0x0400_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
+17.'i_reset' =1 
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector[30:0]' = 0x0800_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 and 'i_r_neg_w' = 0 on the rising edge of 'i_sys_clk'
 2.Set 'i_rs_vector[30:0]' = 0x0000_00000 on the next rising egde of 'i_sys_clk'
 3.Set 'i_rs_vector[30:0]' = 0x1000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 on the next rising edge of 'i_sys_clk'
 4.Set 'i_rs_vector[30:0]' = 0x0000_00000 on the next rising egde of 'i_sys_clk'
@@ -2010,254 +2221,262 @@
 o_tx_w_en,o_hpb_data[127:0],o_hpb_r_en,o_hpb_full,o_acker,o_berr,o_ster,o_fmer,o_crcer
 o_lback,o_sleep,'o_afmr1','o_afmr2','o_afmr3','o_afmr4','o_afir1', 'o_afir2', 'o_afir3', 'o_afir4','o_uaf1','o_uaf2','o_uaf3' and 'o_uaf4'
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.  'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0800_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001  'i_r_neg_w' = 0 '
-2. 'i_rs_vector[30:0]' = 0x0000_00000 
-3. 'i_rs_vector[30:0]' = 0x1000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
-4.'i_rs_vector[30:0]' = 0x0000_00000 
-5.'i_rs_vector[30:0]' = 0x2000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 
-6.'i_rs_vector[30:0]' = 0x0000_00000 
-7.'i_rs_vector[30:0]' = 0x4000_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 
-8.'i_rs_vector[30:0]' = 0x0000_00000 9.'i_rs_vector[30:0]' = 0x0080_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
-10.'i_rs_vector[30:0]' = 0x0000_00000 
-11.'i_rs_vector[30:0]' = 0x0100_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
-12.'i_rs_vector[30:0]' = 0x0000_00000 
-13.'i_rs_vector[30:0]' = 0x0200_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001 
-15.'i_rs_vector[30:0]' = 0x0000_00000
-16.'i_rs_vector[30:0]' = 0x0400_00000 ,'i_reg_w_bus[31:0]' =0x0000_0001
-17.'i_reset' =1 
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Set  'i_rs_vector' to 0x01 
+'i_reg_w_bus[31:0]' =0x2000_0000, 'i_r_neg_w'=0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector' = 0x00 on the 2rd rising edge of 'i_sys_clk' for this test case
+3.Observe 'o_soft_reset' on the 3rd  rising egde of 'i_sys_clk' for this test case.
+4 Observe 'o_soft_reset' on the 4th  rising egde of 'i_sys_clk' for this test case.
+5. Set 'i_reg_w_bus[31:0]' =0x0000_0000
+and 'i_rs_vector' = 0x01  on the 5th rising edge of 'i_sys_clk' for this test case
+6. Set 'i_rs_vector' = 0x00 on the 6th rising edge of 'i_sys_clk' for this test case
+7. observe 'o_soft_reset' on the 7th rising edge of 'i_sys_clk' for this test case
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. i_rs_vector[30:0] = 0x0000_0001
-2. i_rs_vector[30:0] = 0x0000_0000
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector' = 0x01
+ 'i_reg_w_bus[31:0]' =0x2000_0000,
+ 'i_r_neg_w'=0 
+2. 'i_rs_vector' = 0x00
+5. 'i_rs_vector' = 0x01
+ 'i_reg_w_bus[31:0]' =0x0000_0000,
+6. 'i_rs_vector' = 0x00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector[30:0]' = 0x0000_0400 ,'i_reg_w_bus[31:0]' =0x0000_0001, 'i_r_neg_w'=0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_rs_vector{30:0]' to 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Set 'i_rs_vector[30:0]' = 0x0000_0800 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 3rd rising edge of 'i_sys_clk' for this test case
+4. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set 'i_rs_vector[30:0]' = 0x0000_1000 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 5th rising edge of 'i_sys_clk' for this test case
+6. Set 'i_rs_vector' to 0x0000_0000 on the 6th rising edge of 'i_sys_clk' for this test case
+7. Set 'i_rs_vector[30:0]' = 0x0000_2000 ,'i_reg_w_bus[31:0]' =0x0000_0000, on the 7th rising edge of 'i_sys_clk' for this test case
+8. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 8th rising edge of 'i_sys_clk' for this test case
+9. Observe 'o_tx_fifo_data[127:0] on the 9th rising edge of 'i_sys_clk' for this test case
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0020_0000 ,'i_tx_empty'= '0' and 'i_r_neg_w' = 1 on the 1st rising edge of 'i_sys_clk' for this test case
-2.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Observe ‘o_rx_r_en’on the 3rd tising edge of 'i_sys_clk' for this test case.
-4. 'i_rs_vector[30:0]' = 0x0020_0000 ,''i_tx_empty'=1 on the 4th rising edge of 'i_sys_clk' for this test case
-5.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 5th rising edge of 'i_sys_clk' for this test case
-6.Observe ‘o_rx_r_en’ on the 6th tising edge of 'i_sys_clk' for this test case.
-7.'i_rs_vector[30:0]' = 0x0000_0000 ,'i_r_neg_w' = 0 on the 7th rising edge of 'i_sys_clk' for this test case
-8.Observe ‘o_rx_r_en’ on the 9th tising edge of 'i_sys_clk' for this test case.
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.
+ 'i_rs_vector[30:0]' = 0x0000_0400
+ 'i_reg_w_bus[31:0]' =0x0000_0001,
+ 'i_r_neg_w'=0 
+2. 'i_rs_vector[30:0]' = 0x0000_0000
+3.'i_rs_vector[30:0]' = 0x0000_0800
+ 'i_reg_w_bus[31:0]' =0x0000_0001,
+4.'i_rs_vector[30:0]' = 0x0000_0000
+5.'i_rs_vector[30:0]' = 0x0000_1000
+ 'i_reg_w_bus[31:0]' =0x0000_0001,
+6.'i_rs_vector[30:0]' = 0x0000_0000
+7.'i_rs_vector[30:0]' = 0x0000_2000
+ 'i_reg_w_bus[31:0]' =0x0000_0000,
+8..'i_rs_vector[30:0]' = 0x0000_0000
 </t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0020_0000 
-  'i_tx_emptyl'=0 
-  'i_r_neg_w' = 1
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector[30:0]' = 0x0000_2000 ,'i_tx_full'=0 on the 1st rising edge of 'i_sys_clk' for this test case
+2.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 2rd rising edge of 'i_sys_clk' for this test case
+3.Observe 'o_tx_w_en' on the 4th tising edge of 'i_sys_clk' for this test case.
+4. 'i_rs_vector[30:0]' = 0x0000_2000 ,'i_tx_full'=1 on the 5th rising edge of 'i_sys_clk' for this test case
+5.Set  'i_rs_vector[30:0]' = 0x0000_0000  on the 6th rising edge of 'i_sys_clk' for this test case
+6.Observe 'o_tx_w_en' on the 9th tising edge of 'i_sys_clk' for this test case.
+7.'i_rs_vector[30:0]' = 0x0000_0000 ,'i_tx_full'=0 on the 10th rising edge of 'i_sys_clk' for this test case
+8.Observe 'o_tx_w_en' on the 12th tising edge of 'i_sys_clk' for this test case.
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector[30:0]' = 0x0000_2000 
+  'i_tx_full'=0 
 2.'i_rs_vector[30:0]' = 0x0000_0000 
-4,'i_rs_vector[30:0]' = 0x0020_0000 
- 'i_tx_emptyl'=1
+4,'i_rs_vector[30:0]' = 0x0000_2000 
+'i_tx_full'=1 
 5.'i_rs_vector[30:0]' = 0x0000_0000 
 7.'i_rs_vector[30:0]' = 0x0000_0000 
+'i_tx_full'=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set  'i_rs_vector[30:0]' = 0x0000_0400 ,'i_reg_w_bus[31:0]' =0x0000_0001, 'i_r_neg_w'=0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_rs_vector{30:0]' to 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Set 'i_rs_vector[30:0]' = 0x0000_0800 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 3rd rising edge of 'i_sys_clk' for this test case
+4. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set 'i_rs_vector[30:0]' = 0x0001_0000 ,'i_reg_w_bus[31:0]' =0x0000_0001, on the 5th rising edge of 'i_sys_clk' for this test case
+6. Set 'i_rs_vector' to 0x0000_0000 on the 6th rising edge of 'i_sys_clk' for this test case
+7. Set 'i_rs_vector[30:0]' = 0x0002_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000, on the 7th rising edge of 'i_sys_clk' for this test case
+8. Set 'i_rs_vector[30:0]' to 0x0000_0000 on the 8th rising edge of 'i_sys_clk' for this test case
+9. Observe 'o_hpb_data[127:0] on the 9th rising edge of 'i_sys_clk' for this test case
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.
+ 'i_rs_vector[30:0]' = 0x0000_4000
+ 'i_reg_w_bus[31:0]' =0x0000_0001,
+ 'i_r_neg_w'=0 
+2. 'i_rs_vector[30:0]' = 0x0000_0000
+3.'i_rs_vector[30:0]' = 0x0000_8000
+ 'i_reg_w_bus[31:0]' =0x0000_0001,
+4.'i_rs_vector[30:0]' = 0x0000_0000
+5.'i_rs_vector[30:0]' = 0x0001_0000
+ 'i_reg_w_bus[31:0]' =0x0000_0001,
+6.'i_rs_vector[30:0]' = 0x0000_0000
+7.'i_rs_vector[30:0]' = 0x0002_0000
+ 'i_reg_w_bus[31:0]' =0x0000_0000,
+8..'i_rs_vector[30:0]' = 0x0000_0000
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector[30:0]' = 0x0002_0000 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set 'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3,Observe 'o_hpb_r_en' on the 3rd rising edge of 'i_sys_clk' for this test case
+4,Observe 'o_hpb_r_en' on the 4th rising edge of 'i_sys_clk' for this test case
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1
+ 'i_rs_vector[30:0]' = 0x0002_0000 
+2. 'i_rs_vector[30:0]' = 0x0000_0000 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0002_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2.Set 'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_hpb_full' on the 3rd rising edge of 'i_sys_clk' for this test case
+4.Observe 'o_hpb_full' on the 4th rising edge of 'i_sys_clk' for this test case
+5.Set 'i_rs_vector[30:0]' = 0x0002_0000 and 'i_r_neg_w'  = 1 on the 5th rising edge of 'i_sys_clk' for this test case
+6.Observe 'o_hpb_full' on the 7th rising edge of 'i_sys_clk' for this test case</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1
+ 'i_rs_vector[30:0]' = 0x0002_0000
  'i_r_neg_w' = 0
- 'i_tx_emptyl'=1</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x8000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. 'i_rs_vector[30:0]' = 0x0000_0000
+5. 'i_rs_vector[30:0]' = 0x0002_0000
+ 'i_r_neg_w' = 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x4000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
 2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_uaf1' on the 3rd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_lback' on the 3rd rising edge of 'i_can_clk' for this test case
+4. Set  'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6. Observe 'o_lback' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x8000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_sleep' on the 3rd rising edge of 'i_can_clk' for this test case
+4. Set  'i_rs_vector[30:0]' = 0x0000_0002 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6. Observe 'o_sleep' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x1800_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_sjw[1:0]' on the 3rd rising edge of 'i_can_clk' for this test case
+4. Set  'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6. Observe 'o_sjw[1:0]' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0E00_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_ts2[2:0]' on the 3rd rising edge of 'i_can_clk' for this test case
+4. Set  'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6. Observe 'o_ts2[2:0]' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0xF000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_ts1[3:0]' on the 3rd rising edge of 'i_can_clk' for this test case
+4. Set  'i_rs_vector[30:0]' = 0x0000_0004 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
+5. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
+6. Observe 'o_ts1[3:0]' on the 6th  rising edfe of 'i_can_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1. Set  'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
+2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
+3. Observe 'o_uaf4' on the 3rd rising edge of 'i_sys_clk' for this test case
 4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
 5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6 Oberve 'o_uaf1' on the 6th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0040_0000
+6 Observe 'o_uaf4' on the 6th rising edge of 'i_sys_clk' for this test case</t>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector[30:0]' = 0x0000_0004
+ 'i_reg_w_bus[31:0]' =0xF000_0000
+ 'i_r_neg_w' = 0
+2.'i_rs_vector[30:0]' = 0x0000_0000
+4,
+ 'i_rs_vector[30:0]' = 0x0000_0004
+ 'i_reg_w_bus[31:0]' =0x0000_0000
+ 'i_r_neg_w' = 0
+5,'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector[30:0]' = 0x0000_0004
+ 'i_reg_w_bus[31:0]' =0x0E00_0000
+ 'i_r_neg_w' = 0
+2.'i_rs_vector[30:0]' = 0x0000_0000
+4.
+ 'i_rs_vector[30:0]' = 0x0000_0004
+ 'i_reg_w_bus[31:0]' =0x0000_0000
+ 'i_r_neg_w' = 0
+5,'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.
+ 'i_rs_vector[30:0]' = 0x0000_0004
+ 'i_reg_w_bus[31:0]' =0x1800_0000
+ 'i_r_neg_w' = 0
+2.'i_rs_vector[30:0]' = 0x0000_0000
+4,
+ 'i_rs_vector[30:0]' = 0x0000_0004
+ 'i_reg_w_bus[31:0]' =0x0000_0000
+ 'i_r_neg_w' = 0
+5,'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 
+ 'i_rs_vector[30:0]' = 0x0000_0002 
  'i_reg_w_bus[31:0]' =0x8000_0000
  'i_r_neg_w' = 0
 2.'i_rs_vector[30:0]' = 0x0000_0000
-4. 'i_rs_vector[30:0]' = 0x0004_0000 
+4,
+ 'i_rs_vector[30:0]' = 0x0000_0002 
  'i_reg_w_bus[31:0]' =0x0000_0000
  'i_r_neg_w' = 0
-5.'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x4000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_uaf2' on the 3rd rising edge of 'i_sys_clk' for this test case
-4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6 Oberve 'o_uaf2' on the 6th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0040_0000
+5,'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 
+ 'i_rs_vector[30:0]' = 0x0000_0002 
  'i_reg_w_bus[31:0]' =0x4000_0000
  'i_r_neg_w' = 0
 2.'i_rs_vector[30:0]' = 0x0000_0000
-4. 'i_rs_vector[30:0]' = 0x0004_0000 
+4,
+ 'i_rs_vector[30:0]' = 0x0000_0002 
  'i_reg_w_bus[31:0]' =0x0000_0000
  'i_r_neg_w' = 0
-5.'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x2000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_uaf3' on the 3rd rising edge of 'i_sys_clk' for this test case
-4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6 Oberve 'o_uaf3' on the 6th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0040_0000
- 'i_reg_w_bus[31:0]' =0x2000_0000
- 'i_r_neg_w' = 0
-2.'i_rs_vector[30:0]' = 0x0000_0000
-4. 'i_rs_vector[30:0]' = 0x0004_0000 
- 'i_reg_w_bus[31:0]' =0x0000_0000
- 'i_r_neg_w' = 0
-5.'i_rs_vector[30:0]' = 0x0000_0000</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0800_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afmr1' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x0800_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x1000_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afmr2' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x1000_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x2000_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afmr3' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x2000_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x4000_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afmr4' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x4000_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0080_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afir1' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x0080_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0100_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afir2' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x0100_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0200_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afir3' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x0200_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 1'  on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set 'i_reset = 0' ,'i_rs_vector[30:0]' = 0x0400_00000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0  on the 2nd rising edge of 'i_sys_clk' for this test case
-3.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 3rd rising edge of 'i_sys_clk' for this test case
-4 Oberve 'o_afir4' on the 4th rising edge of 'i_sys_clk' for this test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.'i_reset = 1 
-2.  'i_reset = 0' 
-    'i_rs_vector[30:0]' = 0x0400_0000 ,
-   'i_reg_w_bus[31:0]' =0x1000_0000          'i_r_neg_w' = 0
-3.'i_rs_vector[30:0]' = 0x0000_000 ,
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The internal register,
- rx DLC[31:0], stores the value,‘i_rx_fifo_data[95:64]’, when ‘o_rx_r_en’ is 1 and ‘i_sys_clk’ transitions from 0 to 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The internal register,
- rx DW1[31:0], stores the value,‘i_rx_fifo_data[63:32]’, when ‘o_rx_r_en’ is 1 and ‘i_sys_clk’ transitions from 0 to 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The internal register,
- rx DW2[31:0], stores the value,‘i_rx_fifo_data[31:0]’, when ‘o_rx_r_en’ is 1 and ‘i_sys_clk’ transitions from 0 to 1.</t>
-  </si>
-  <si>
-    <t>1. 'i_reset = 0'
- 'i_rs_vector[30:0]' = 0x0040_0000
- 'i_reg_w_bus[31:0]' =0x1000_0000
- 'i_r_neg_w' = 0
-2.'i_rs_vector[30:0]' = 0x0000_0000
-4. 'i_rs_vector[30:0]' = 0x0004_0000 
- 'i_reg_w_bus[31:0]' =0x0000_0000
- 'i_r_neg_w' = 0
-5.'i_rs_vector[30:0]' = 0x0000_0000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Set 'i_reset = 0', 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x1000_0000 and 'i_r_neg_w' = 0 on the 1st rising edge of 'i_sys_clk' for this test case
-2. Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 2nd rising edge of 'i_sys_clk' for this test case
-3. Oberve 'o_uaf4' on the 3rd rising edge of 'i_sys_clk' for this test case
-4. 'i_rs_vector[30:0]' = 0x0040_0000 ,'i_reg_w_bus[31:0]' =0x0000_0000 and 'i_r_neg_w' = 0 on the 4th rising edge of 'i_sys_clk' for this test case
-5.Set  'i_rs_vector[30:0]' = 0x0000_0000 on the 5th rising edge of 'i_sys_clk' for this test case
-6 Oberve 'o_uaf4' on the 6th rising edge of 'i_sys_clk' for this test case</t>
+5,'i_rs_vector[30:0]' = 0x0000_0000</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2339,6 +2558,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Antonio Jimenez" id="{0742E221-2625-40A9-AAF8-BB523327651B}" userId="c97ae766613fd935" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2602,25 +2827,72 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D3" dT="2020-07-23T20:40:16.93" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{B9A5ACC3-A9D2-4160-8B01-ED5E40C7E189}">
+    <text>Change observe</text>
+  </threadedComment>
+  <threadedComment ref="F3" dT="2020-07-23T20:39:38.95" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{5A482186-F8B0-4721-BAB6-AA12B84DC195}">
+    <text>Switch step 3 and 4 results</text>
+  </threadedComment>
+  <threadedComment ref="D5" dT="2020-07-23T15:37:58.34" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{5489723F-98BE-48A3-9BEE-41627AB309AB}">
+    <text>what is i_rs_vector 0x07 supposed to be?</text>
+  </threadedComment>
+  <threadedComment ref="E5" dT="2020-07-23T20:42:09.66" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{24497671-CD24-42BA-A892-1D9B4829AD51}">
+    <text>Change 0x07</text>
+  </threadedComment>
+  <threadedComment ref="D12" dT="2020-07-23T20:10:04.91" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{4000C2C9-1249-4C51-ABEA-466F92E1810B}">
+    <text>Observe is spelled wrong</text>
+  </threadedComment>
+  <threadedComment ref="D13" dT="2020-07-23T20:11:45.59" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{E98452AD-1B41-492A-B6A6-FF2BFA437ADE}">
+    <text>Observe spelled wrong</text>
+  </threadedComment>
+  <threadedComment ref="D16" dT="2020-07-23T20:19:02.56" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{A89E9DD6-6233-400D-A1D8-3EA3584E1725}">
+    <text>Observe spelled wrong</text>
+  </threadedComment>
+  <threadedComment ref="D16" dT="2020-07-23T20:19:42.80" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{FC883704-623A-4CAC-B85D-28EE2F1C4CD1}" parentId="{A89E9DD6-6233-400D-A1D8-3EA3584E1725}">
+    <text>You set i_reset to 0 two times here</text>
+  </threadedComment>
+  <threadedComment ref="D18" dT="2020-07-23T20:22:53.22" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{1DD4B513-0EC7-472B-AA76-F7140FE48B4E}">
+    <text>observe</text>
+  </threadedComment>
+  <threadedComment ref="D19" dT="2020-07-23T20:22:57.51" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{B32CBE22-EA4E-4B50-9220-DFCBAD24D24C}">
+    <text>observe</text>
+  </threadedComment>
+  <threadedComment ref="E19" dT="2020-07-23T20:23:58.28" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{1AE28864-5635-48BA-A24C-742FBA5CB0F2}">
+    <text>4. needs to be written as 0x00040_0000</text>
+  </threadedComment>
+  <threadedComment ref="D20" dT="2020-07-23T20:24:32.30" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{C02CFA98-42BE-4FB7-88D5-81435EDA7417}">
+    <text>Observe</text>
+  </threadedComment>
+  <threadedComment ref="E20" dT="2020-07-23T20:24:24.33" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{67C72576-4EBB-4155-8BBD-0EFDB0C573B9}">
+    <text>4. 0x0040_0000</text>
+  </threadedComment>
+  <threadedComment ref="D30" dT="2020-07-23T20:29:14.21" personId="{0742E221-2625-40A9-AAF8-BB523327651B}" id="{C8BA079A-770E-4D28-A0A8-7EC7E1AE781E}">
+    <text>you don't specify that i_Reset was ever 1</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18.58203125" customWidth="1"/>
-    <col min="4" max="4" width="77.08203125" customWidth="1"/>
+    <col min="4" max="4" width="77.1640625" customWidth="1"/>
     <col min="5" max="5" width="32.25" customWidth="1"/>
     <col min="6" max="6" width="33.1640625" customWidth="1"/>
     <col min="7" max="7" width="14.4140625" customWidth="1"/>
     <col min="8" max="8" width="16.75" customWidth="1"/>
-    <col min="9" max="9" width="16.9140625" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2663,13 +2935,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>318</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="313" customHeight="1" x14ac:dyDescent="0.3">
@@ -2677,1204 +2949,1205 @@
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>319</v>
+        <v>260</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>341</v>
+        <v>236</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="295.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>251</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>252</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>254</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>272</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>271</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>351</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>352</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>255</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>354</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="332.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>322</v>
+        <v>355</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>323</v>
+        <v>356</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>44</v>
+        <v>258</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>324</v>
+        <v>357</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>45</v>
+        <v>358</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="159" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>325</v>
+        <v>359</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>326</v>
+        <v>360</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="235" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
+        <v>259</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>327</v>
+        <v>361</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>328</v>
+        <v>362</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="253" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>329</v>
+        <v>363</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>330</v>
+        <v>373</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="274" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>332</v>
+        <v>372</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="245.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>333</v>
+        <v>365</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="286.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>335</v>
+        <v>366</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="268" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>337</v>
+        <v>367</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>338</v>
+        <v>369</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="308.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="268" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="235.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>346</v>
+        <v>276</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="242.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>348</v>
+        <v>277</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>349</v>
+        <v>279</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="285.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="285.64999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>369</v>
+        <v>278</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="236.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>350</v>
+        <v>261</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>351</v>
+        <v>237</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="209.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>352</v>
+        <v>262</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>353</v>
+        <v>238</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="186" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>354</v>
+        <v>263</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>355</v>
+        <v>239</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="170.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>356</v>
+        <v>264</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>357</v>
+        <v>240</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="183" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>358</v>
+        <v>265</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>359</v>
+        <v>241</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="187.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>360</v>
+        <v>266</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>361</v>
+        <v>242</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="192.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="192.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>362</v>
+        <v>267</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>363</v>
+        <v>243</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="177.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="177.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>364</v>
+        <v>268</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>365</v>
+        <v>244</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="164" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="164.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>135</v>
+        <v>280</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>129</v>
+        <v>281</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>366</v>
+        <v>245</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>134</v>
+        <v>282</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>129</v>
+        <v>283</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="164" customHeight="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="164.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>367</v>
+        <v>246</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>139</v>
+        <v>343</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>129</v>
+        <v>342</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>368</v>
+        <v>247</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>143</v>
+        <v>341</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>129</v>
+        <v>340</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="119" customHeight="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="119.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>150</v>
+        <v>336</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>148</v>
+        <v>339</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>154</v>
+        <v>337</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>155</v>
+        <v>338</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>171</v>
+        <v>284</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>163</v>
+        <v>285</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>170</v>
+        <v>286</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>165</v>
+        <v>287</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="105.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="105.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>172</v>
+        <v>288</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="204" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>182</v>
+        <v>289</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>178</v>
+        <v>290</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="207" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>184</v>
+        <v>291</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>185</v>
+        <v>292</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="229" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>193</v>
+        <v>293</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>196</v>
+        <v>294</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="219.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="219.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>195</v>
+        <v>295</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>197</v>
+        <v>296</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="178.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>202</v>
+        <v>297</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>203</v>
+        <v>298</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="166.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>207</v>
+        <v>162</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>208</v>
+        <v>299</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>209</v>
+        <v>300</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>210</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>212</v>
+        <v>165</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>213</v>
+        <v>166</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>214</v>
+        <v>301</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>215</v>
+        <v>302</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>218</v>
+        <v>169</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>219</v>
+        <v>170</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>220</v>
+        <v>303</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>221</v>
+        <v>304</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="164.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>225</v>
+        <v>174</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>226</v>
+        <v>305</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>227</v>
+        <v>306</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="226.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>230</v>
+        <v>177</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>232</v>
+        <v>307</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>233</v>
+        <v>308</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="185.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>238</v>
+        <v>309</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>215</v>
+        <v>302</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>239</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="175" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>240</v>
+        <v>184</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>241</v>
+        <v>185</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>242</v>
+        <v>186</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>243</v>
+        <v>310</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>244</v>
+        <v>311</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>245</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="207" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>246</v>
+        <v>188</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>248</v>
+        <v>190</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>250</v>
+        <v>313</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>251</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="172" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>252</v>
+        <v>192</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>253</v>
+        <v>193</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>254</v>
+        <v>194</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>256</v>
+        <v>315</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>257</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="169" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>258</v>
+        <v>196</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>259</v>
+        <v>197</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>260</v>
+        <v>198</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>261</v>
+        <v>316</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>262</v>
+        <v>317</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="224" customHeight="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="224.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>264</v>
+        <v>200</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>265</v>
+        <v>201</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>267</v>
+        <v>318</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="241" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>270</v>
+        <v>204</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>271</v>
+        <v>205</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>272</v>
+        <v>206</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>274</v>
+        <v>321</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>275</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="181.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>276</v>
+        <v>208</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>277</v>
+        <v>209</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>283</v>
+        <v>213</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>278</v>
+        <v>322</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>279</v>
+        <v>323</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="219.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="219.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>281</v>
+        <v>211</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>284</v>
+        <v>214</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>287</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>288</v>
+        <v>216</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>289</v>
+        <v>217</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>290</v>
+        <v>218</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>297</v>
+        <v>326</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>291</v>
+        <v>327</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>292</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="227.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>294</v>
+        <v>221</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>298</v>
+        <v>329</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="195" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>301</v>
+        <v>225</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>302</v>
+        <v>226</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>305</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="230.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>306</v>
+        <v>228</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>307</v>
+        <v>229</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>308</v>
+        <v>230</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="197" customHeight="1" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="197.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>312</v>
+        <v>232</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>313</v>
+        <v>233</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>314</v>
+        <v>234</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>317</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CAN1-68 Configuration Test cases V3
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/configuration _register_test_cases.xlsx
+++ b/Documentations/Test Cases/configuration _register_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hruy1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D1E4C-84C2-4B69-8E77-D98021DC18C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111427E4-7924-417E-98AA-684C58696138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1597,27 +1597,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1.
- 'i_rs_vector' = 0x07
- 'i_reg_w_bus[31:0]' =0x00,
- 'i_r_neg_w'=0 
- 'i_sleep' = 1 
-3.'i_reg_w_bus[31:0]' =0x0020_0000
-5.'i_sleep' = 0
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Set 'i_rs_vector' to 0x07 'i_reg_w_bus[31:0]' =0x00, 'i_r_neg_w'=0 and 'i_sleep' = 1 on the 1st rising edge of 'i_sys_clk' for this test case
-2 Observe 'o_interrupt' on the 4th  rising egde of 'i_sys_clk' for this test case.
-3.Set  'i_rs_vector' to 0x80 'i_reg_w_bus[31:0]' =0x0020_0000, 'i_r_neg_w'=0  on the 5th rising edge of 'i_sys_clk' for this test case
-4.Observe 'o_interrupt' on the 9th rising egde of 'i_sys_clk' for this test case.
-5. Set 'i_sleep' = 0 ont the 10th rirsing edge of 'i_sys_clk' for this test case
-6.Observe 'o_interrupt' on the 13th rising egde of 'i_sys_clk' for this test case.
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Step 2: 
 'o_interrupt'  = 0
 Step 4: 
@@ -2477,6 +2456,27 @@
  'i_reg_w_bus[31:0]' =0x0000_0000
  'i_r_neg_w' = 0
 5,'i_rs_vector[30:0]' = 0x0000_0000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Set 'i_rs_vector' to 0x80 'i_reg_w_bus[31:0]' =0x00, 'i_r_neg_w'=0 and 'i_sleep' = 1 on the 1st rising edge of 'i_sys_clk' for this test case
+2 Observe 'o_interrupt' on the 4th  rising egde of 'i_sys_clk' for this test case.
+3.Set  'i_rs_vector' to 0x80 'i_reg_w_bus[31:0]' =0x0020_0000, 'i_r_neg_w'=0  on the 5th rising edge of 'i_sys_clk' for this test case
+4.Observe 'o_interrupt' on the 9th rising egde of 'i_sys_clk' for this test case.
+5. Set 'i_sleep' = 0 ont the 10th rirsing edge of 'i_sys_clk' for this test case
+6.Observe 'o_interrupt' on the 13th rising egde of 'i_sys_clk' for this test case.
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.
+ 'i_rs_vector' = 0x80
+ 'i_reg_w_bus[31:0]' =0x00,
+ 'i_r_neg_w'=0 
+ 'i_sleep' = 1 
+3.'i_reg_w_bus[31:0]' =0x0020_0000
+5.'i_sleep' = 0
+</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2878,8 +2878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2935,10 +2935,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>248</v>
@@ -2995,13 +2995,13 @@
         <v>254</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>272</v>
+        <v>372</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3015,10 +3015,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
@@ -3035,10 +3035,10 @@
         <v>255</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>256</v>
@@ -3055,10 +3055,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>26</v>
@@ -3075,10 +3075,10 @@
         <v>258</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>257</v>
@@ -3095,13 +3095,13 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="235" customHeight="1" x14ac:dyDescent="0.3">
@@ -3115,13 +3115,13 @@
         <v>259</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="253" customHeight="1" x14ac:dyDescent="0.3">
@@ -3135,10 +3135,10 @@
         <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>40</v>
@@ -3155,10 +3155,10 @@
         <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>41</v>
@@ -3175,10 +3175,10 @@
         <v>44</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>45</v>
@@ -3195,10 +3195,10 @@
         <v>48</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>49</v>
@@ -3215,10 +3215,10 @@
         <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>369</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>53</v>
@@ -3235,10 +3235,10 @@
         <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>57</v>
@@ -3255,10 +3255,10 @@
         <v>60</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>64</v>
@@ -3275,10 +3275,10 @@
         <v>63</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>65</v>
@@ -3295,10 +3295,10 @@
         <v>68</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>69</v>
@@ -3315,10 +3315,10 @@
         <v>72</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>73</v>
@@ -3495,10 +3495,10 @@
         <v>111</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>108</v>
@@ -3515,10 +3515,10 @@
         <v>245</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>112</v>
@@ -3535,10 +3535,10 @@
         <v>246</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>115</v>
@@ -3555,10 +3555,10 @@
         <v>247</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>118</v>
@@ -3575,10 +3575,10 @@
         <v>121</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>122</v>
@@ -3595,10 +3595,10 @@
         <v>125</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>126</v>
@@ -3615,10 +3615,10 @@
         <v>132</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>129</v>
@@ -3635,10 +3635,10 @@
         <v>133</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>134</v>
@@ -3655,7 +3655,7 @@
         <v>137</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>138</v>
@@ -3675,10 +3675,10 @@
         <v>142</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>146</v>
@@ -3695,10 +3695,10 @@
         <v>145</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>147</v>
@@ -3715,10 +3715,10 @@
         <v>149</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>150</v>
@@ -3735,10 +3735,10 @@
         <v>154</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>155</v>
@@ -3755,10 +3755,10 @@
         <v>158</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>159</v>
@@ -3775,10 +3775,10 @@
         <v>162</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>163</v>
@@ -3795,10 +3795,10 @@
         <v>166</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>167</v>
@@ -3815,10 +3815,10 @@
         <v>170</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>171</v>
@@ -3835,10 +3835,10 @@
         <v>174</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>175</v>
@@ -3855,10 +3855,10 @@
         <v>178</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>179</v>
@@ -3875,10 +3875,10 @@
         <v>182</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>183</v>
@@ -3895,10 +3895,10 @@
         <v>186</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>187</v>
@@ -3915,10 +3915,10 @@
         <v>190</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>191</v>
@@ -3935,10 +3935,10 @@
         <v>194</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>195</v>
@@ -3955,10 +3955,10 @@
         <v>198</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>199</v>
@@ -3975,10 +3975,10 @@
         <v>202</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>203</v>
@@ -3995,10 +3995,10 @@
         <v>206</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>207</v>
@@ -4015,10 +4015,10 @@
         <v>213</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>210</v>
@@ -4035,10 +4035,10 @@
         <v>214</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>215</v>
@@ -4055,10 +4055,10 @@
         <v>218</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>219</v>
@@ -4075,10 +4075,10 @@
         <v>222</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>223</v>
@@ -4095,10 +4095,10 @@
         <v>226</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>227</v>
@@ -4115,10 +4115,10 @@
         <v>230</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>231</v>
@@ -4135,10 +4135,10 @@
         <v>234</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>235</v>

</xml_diff>